<commit_message>
feat: Adição de rodapé com informações úteis
Implementado rodapé informativo contendo logotipos dos apoiadores e informações do desenvolvedor.
</commit_message>
<xml_diff>
--- a/relatorio_promar.xlsx
+++ b/relatorio_promar.xlsx
@@ -46,13 +46,13 @@
     <t>b-o vento</t>
   </si>
   <si>
-    <t>b-Um ser humano</t>
-  </si>
-  <si>
     <t>b-Carros</t>
   </si>
   <si>
     <t>b-Brincando na praia</t>
+  </si>
+  <si>
+    <t>a-Um animal</t>
   </si>
   <si>
     <t>Cidades com Melhor Desempenho</t>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -482,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -490,7 +490,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -498,7 +498,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -506,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -514,7 +514,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -535,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -564,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -601,7 +601,7 @@
         <v>21</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2">

</xml_diff>

<commit_message>
refator: Alterando a view relatóroi para receber filtro por ês
</commit_message>
<xml_diff>
--- a/relatorio_promar.xlsx
+++ b/relatorio_promar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Categoria</t>
   </si>
@@ -43,10 +43,7 @@
     <t>b-Casa para os peixes</t>
   </si>
   <si>
-    <t>b-o vento</t>
-  </si>
-  <si>
-    <t>b-Carros</t>
+    <t>b-Um ser humano</t>
   </si>
   <si>
     <t>b-Brincando na praia</t>
@@ -55,6 +52,12 @@
     <t>a-Um animal</t>
   </si>
   <si>
+    <t>c-Olhando os peixes</t>
+  </si>
+  <si>
+    <t>a-Não jogando lixo nele</t>
+  </si>
+  <si>
     <t>Cidades com Melhor Desempenho</t>
   </si>
   <si>
@@ -82,10 +85,13 @@
     <t>10-12</t>
   </si>
   <si>
+    <t>5-7</t>
+  </si>
+  <si>
+    <t>mais_de_12</t>
+  </si>
+  <si>
     <t>7-9</t>
-  </si>
-  <si>
-    <t>5-7</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,7 +451,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -461,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -482,7 +488,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -514,28 +520,28 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>5</v>
+      <c r="B16" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -543,80 +549,104 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
         <v>2</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B29">
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refator: Resolvido o problema de não imprimir por mês
</commit_message>
<xml_diff>
--- a/relatorio_promar.xlsx
+++ b/relatorio_promar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Categoria</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>July</t>
+    <t>June</t>
   </si>
   <si>
     <t>Total de Visitantes</t>
@@ -46,36 +46,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>b-Casa para os peixes</t>
-  </si>
-  <si>
-    <t>b-Um ser humano</t>
-  </si>
-  <si>
-    <t>b-Brincando na praia</t>
-  </si>
-  <si>
-    <t>a-Um animal</t>
-  </si>
-  <si>
-    <t>c-Olhando os peixes</t>
-  </si>
-  <si>
-    <t>a-Não jogando lixo nele</t>
-  </si>
-  <si>
     <t>Cidades com Melhor Desempenho</t>
   </si>
   <si>
     <t>Cidade</t>
   </si>
   <si>
-    <t>Vera Cruz</t>
-  </si>
-  <si>
-    <t>Itaparica</t>
-  </si>
-  <si>
     <t>Notas Mais Dadas</t>
   </si>
   <si>
@@ -86,18 +62,6 @@
   </si>
   <si>
     <t>Idade</t>
-  </si>
-  <si>
-    <t>10-12</t>
-  </si>
-  <si>
-    <t>5-7</t>
-  </si>
-  <si>
-    <t>mais_de_12</t>
-  </si>
-  <si>
-    <t>7-9</t>
   </si>
 </sst>
 </file>
@@ -438,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -473,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -481,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -497,171 +461,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refator: Adicionado formatação nas tabelas
</commit_message>
<xml_diff>
--- a/relatorio_promar.xlsx
+++ b/relatorio_promar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Categoria</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>June</t>
+    <t>Julho</t>
   </si>
   <si>
     <t>Total de Visitantes</t>
@@ -46,12 +46,36 @@
     <t>Total</t>
   </si>
   <si>
+    <t>b-Casa para os peixes</t>
+  </si>
+  <si>
+    <t>b-Um ser humano</t>
+  </si>
+  <si>
+    <t>b-Brincando na praia</t>
+  </si>
+  <si>
+    <t>a-Um animal</t>
+  </si>
+  <si>
+    <t>c-Olhando os peixes</t>
+  </si>
+  <si>
+    <t>a-Não jogando lixo nele</t>
+  </si>
+  <si>
     <t>Cidades com Melhor Desempenho</t>
   </si>
   <si>
     <t>Cidade</t>
   </si>
   <si>
+    <t>Vera Cruz</t>
+  </si>
+  <si>
+    <t>Itaparica</t>
+  </si>
+  <si>
     <t>Notas Mais Dadas</t>
   </si>
   <si>
@@ -62,6 +86,18 @@
   </si>
   <si>
     <t>Idade</t>
+  </si>
+  <si>
+    <t>10-12</t>
+  </si>
+  <si>
+    <t>5-7</t>
+  </si>
+  <si>
+    <t>mais_de_12</t>
+  </si>
+  <si>
+    <t>7-9</t>
   </si>
 </sst>
 </file>
@@ -85,15 +121,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,13 +149,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,13 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="20" customHeight="1"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,88 +490,216 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" ht="20" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B4" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" ht="20" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:2" ht="20" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="18" spans="1:2" ht="20" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="23" spans="1:2" ht="20" customHeight="1">
+      <c r="A23" s="2">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20" customHeight="1">
+      <c r="A24" s="2">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20" customHeight="1">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20" customHeight="1">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Adicionado vídeos do ambiente marinho na área do visitante
</commit_message>
<xml_diff>
--- a/relatorio_promar.xlsx
+++ b/relatorio_promar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Categoria</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>Julho</t>
+    <t>Agosto</t>
   </si>
   <si>
     <t>Total de Visitantes</t>
@@ -46,36 +46,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>b-Casa para os peixes</t>
-  </si>
-  <si>
-    <t>b-Um ser humano</t>
-  </si>
-  <si>
-    <t>b-Brincando na praia</t>
-  </si>
-  <si>
-    <t>a-Um animal</t>
-  </si>
-  <si>
-    <t>c-Olhando os peixes</t>
-  </si>
-  <si>
-    <t>a-Não jogando lixo nele</t>
-  </si>
-  <si>
     <t>Cidades com Melhor Desempenho</t>
   </si>
   <si>
     <t>Cidade</t>
   </si>
   <si>
-    <t>Vera Cruz</t>
-  </si>
-  <si>
-    <t>Itaparica</t>
-  </si>
-  <si>
     <t>Notas Mais Dadas</t>
   </si>
   <si>
@@ -86,18 +62,6 @@
   </si>
   <si>
     <t>Idade</t>
-  </si>
-  <si>
-    <t>10-12</t>
-  </si>
-  <si>
-    <t>5-7</t>
-  </si>
-  <si>
-    <t>mais_de_12</t>
-  </si>
-  <si>
-    <t>7-9</t>
   </si>
 </sst>
 </file>
@@ -473,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" customHeight="1">
@@ -511,7 +475,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" customHeight="1">
@@ -519,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20" customHeight="1">
@@ -535,171 +499,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20" customHeight="1">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2" ht="20" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20" customHeight="1">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="20" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="20" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="20" customHeight="1">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="20" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="20" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="20" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="20" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="20" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="20" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="20" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="20" customHeight="1">
-      <c r="A23" s="2">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="20" customHeight="1">
-      <c r="A24" s="2">
-        <v>8</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="20" customHeight="1">
-      <c r="A25" s="2">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="20" customHeight="1">
-      <c r="A26" s="2">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="20" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="20" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="20" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="20" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="20" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="20" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>